<commit_message>
mapping colors, choses.py upgrades, main.loop
</commit_message>
<xml_diff>
--- a/output/planilhas/leilaoimoveis_eusebio-ce.xlsx
+++ b/output/planilhas/leilaoimoveis_eusebio-ce.xlsx
@@ -538,7 +538,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -578,7 +578,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -586,15 +586,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>8083</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>37178</t>
-        </is>
+      <c r="Q2" t="n">
+        <v>8083</v>
+      </c>
+      <c r="R2" t="n">
+        <v>37178</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -610,7 +606,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -648,7 +644,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -656,15 +652,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>9288</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q3" t="n">
+        <v>9288</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -680,7 +672,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -722,7 +714,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -730,15 +722,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>9886</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q4" t="n">
+        <v>9886</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -754,7 +742,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -794,7 +782,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -802,15 +790,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
@@ -826,7 +810,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -868,7 +852,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -876,15 +860,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>9010</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q6" t="n">
+        <v>9010</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -900,7 +880,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -942,7 +922,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -950,15 +930,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>17516</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q7" t="n">
+        <v>17516</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -974,7 +950,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1016,7 +992,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1024,15 +1000,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>10329</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>38155</t>
-        </is>
+      <c r="Q8" t="n">
+        <v>10329</v>
+      </c>
+      <c r="R8" t="n">
+        <v>38155</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
@@ -1048,7 +1020,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1090,7 +1062,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1098,15 +1070,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>10292</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>40372</t>
-        </is>
+      <c r="Q9" t="n">
+        <v>10292</v>
+      </c>
+      <c r="R9" t="n">
+        <v>40372</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
@@ -1122,7 +1090,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1164,7 +1132,7 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1172,15 +1140,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>53395</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>000051204</t>
-        </is>
+      <c r="Q10" t="n">
+        <v>53395</v>
+      </c>
+      <c r="R10" t="n">
+        <v>51204</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -1196,7 +1160,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1234,7 +1198,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1242,15 +1206,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>17494</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q11" t="n">
+        <v>17494</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -1266,7 +1226,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1308,7 +1268,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1316,15 +1276,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>21556</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q12" t="n">
+        <v>21556</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -1340,7 +1296,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1382,7 +1338,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1390,15 +1346,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>21729</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q13" t="n">
+        <v>21729</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
@@ -1414,7 +1366,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1454,7 +1406,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1462,15 +1414,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>21682</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q14" t="n">
+        <v>21682</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
@@ -1486,7 +1434,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1526,7 +1474,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1534,15 +1482,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>21470</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q15" t="n">
+        <v>21470</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
@@ -1558,7 +1502,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1600,7 +1544,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1608,15 +1552,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>17623</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q16" t="n">
+        <v>17623</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -1632,7 +1572,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1674,7 +1614,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1682,15 +1622,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>21658</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q17" t="n">
+        <v>21658</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
@@ -1706,7 +1642,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1748,7 +1684,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1756,15 +1692,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>21493</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q18" t="n">
+        <v>21493</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
@@ -1780,7 +1712,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1822,7 +1754,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1830,15 +1762,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>21509</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q19" t="n">
+        <v>21509</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
@@ -1854,7 +1782,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1896,7 +1824,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1904,15 +1832,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>16772</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q20" t="n">
+        <v>16772</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
@@ -1928,7 +1852,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1968,7 +1892,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -1976,15 +1900,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>8982</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q21" t="n">
+        <v>8982</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2000,7 +1920,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -2042,7 +1962,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2050,15 +1970,11 @@
           <t xml:space="preserve"> Leilão Caixa </t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>8567</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>37002</t>
-        </is>
+      <c r="Q22" t="n">
+        <v>8567</v>
+      </c>
+      <c r="R22" t="n">
+        <v>37002</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2074,7 +1990,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -2106,7 +2022,7 @@
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
-          <t>VendaDiretaCaixa</t>
+          <t>Venda Direta Caixa</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2115,15 +2031,11 @@
 </t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>6870</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>0103009196900000</t>
-        </is>
+      <c r="Q23" t="n">
+        <v>6870</v>
+      </c>
+      <c r="R23" t="n">
+        <v>103009196900000</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2139,7 +2051,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2187,15 +2099,11 @@
           <t xml:space="preserve"> Baldissera Leiloeiros </t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>9273</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q24" t="n">
+        <v>9273</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2211,7 +2119,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2251,7 +2159,7 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2259,15 +2167,11 @@
           <t xml:space="preserve"> GP Leilões </t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>10845</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>40768</t>
-        </is>
+      <c r="Q25" t="n">
+        <v>10845</v>
+      </c>
+      <c r="R25" t="n">
+        <v>40768</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -2283,7 +2187,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -2325,7 +2229,7 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2333,15 +2237,11 @@
           <t xml:space="preserve"> O Leilões </t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>8272</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q26" t="n">
+        <v>8272</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
@@ -2357,7 +2257,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Apartamento </t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -2399,7 +2299,7 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>LeilãoSFICaixa</t>
+          <t>Leilão SFI Caixa</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2407,15 +2307,11 @@
           <t xml:space="preserve"> Rocha Leilões </t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>23862</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>0101000000100431</t>
-        </is>
+      <c r="Q27" t="n">
+        <v>23862</v>
+      </c>
+      <c r="R27" t="n">
+        <v>101000000100431</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
@@ -2431,7 +2327,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Casa </t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -2461,7 +2357,7 @@
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
-          <t>VendaDireta</t>
+          <t>Venda Direta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2483,7 +2379,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Terreno </t>
+          <t>Terreno</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -2513,7 +2409,7 @@
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
-          <t>VendaDireta</t>
+          <t>Venda Direta</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2539,7 +2435,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Outros </t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -2569,7 +2465,7 @@
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr">
         <is>
-          <t>VendaDireta</t>
+          <t>Venda Direta</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2595,7 +2491,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Terreno </t>
+          <t>Terreno</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -2627,7 +2523,7 @@
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr">
         <is>
-          <t>VendaDireta</t>
+          <t>Venda Direta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">

</xml_diff>